<commit_message>
fix: Types of meal percentages
</commit_message>
<xml_diff>
--- a/src/static/doc/type_of_meal.xlsx
+++ b/src/static/doc/type_of_meal.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -294,11 +294,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -314,6 +315,11 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -358,8 +364,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -383,10 +393,10 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.27"/>
@@ -427,10 +437,10 @@
         <v>30</v>
       </c>
       <c r="D2" s="0" t="n">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E2" s="0" t="n">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="F2" s="0" t="s">
         <v>7</v>
@@ -444,13 +454,13 @@
         <v>50</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>40</v>
-      </c>
-      <c r="D3" s="0" t="n">
-        <v>60</v>
-      </c>
-      <c r="E3" s="0" t="n">
         <v>30</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="E3" s="1" t="n">
+        <v>55</v>
       </c>
       <c r="F3" s="0" t="s">
         <v>9</v>
@@ -478,7 +488,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="71.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.75"/>

</xml_diff>